<commit_message>
documento de layout completo e ajustes na controller estudante
</commit_message>
<xml_diff>
--- a/Layout-import.xlsx
+++ b/Layout-import.xlsx
@@ -13,15 +13,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t xml:space="preserve">00ZOOLOGICO27-05-2021 23:04:2201</t>
   </si>
   <si>
-    <t xml:space="preserve">01 100true 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02  102</t>
+    <t xml:space="preserve">01 100true 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02   102</t>
+  </si>
+  <si>
+    <t>12345678901234567890123456789012345</t>
   </si>
   <si>
     <t xml:space="preserve">03doce      maça do amor 10 10.00</t>
@@ -30,6 +33,9 @@
     <t>0400003</t>
   </si>
   <si>
+    <t xml:space="preserve">Tamanho dados uteis:32</t>
+  </si>
+  <si>
     <t xml:space="preserve">Número do campo</t>
   </si>
   <si>
@@ -108,7 +114,10 @@
     <t xml:space="preserve">versionamento de arquivo</t>
   </si>
   <si>
-    <t xml:space="preserve">registro ingresso adulto: "01"</t>
+    <t xml:space="preserve">Tamanho dados uteis:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registro ingresso adulto: "02"</t>
   </si>
   <si>
     <t xml:space="preserve">quantidade de ingressos</t>
@@ -117,7 +126,7 @@
     <t>005</t>
   </si>
   <si>
-    <t>003-008</t>
+    <t>003-007</t>
   </si>
   <si>
     <t xml:space="preserve">Quantidade de ingressos adultos comprados</t>
@@ -126,7 +135,7 @@
     <t>premium</t>
   </si>
   <si>
-    <t>009-014</t>
+    <t>008-012</t>
   </si>
   <si>
     <t>l</t>
@@ -141,16 +150,16 @@
     <t>001</t>
   </si>
   <si>
-    <t>015-015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ingresso adulto: "1"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">registro ingresso estudante: "02"</t>
-  </si>
-  <si>
-    <t>003-007</t>
+    <t>013-013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ingresso adulto: "3"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamanho dados uteis:8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registro ingresso estudante: "03"</t>
   </si>
   <si>
     <t xml:space="preserve">Quantidade de ingressos estudantes comprados</t>
@@ -162,7 +171,10 @@
     <t xml:space="preserve">ingresso estudante: "2"</t>
   </si>
   <si>
-    <t xml:space="preserve">registro produto: "03"</t>
+    <t xml:space="preserve">Tamanho dados uteis:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registro produto: "04"</t>
   </si>
   <si>
     <t xml:space="preserve">tipo de produto</t>
@@ -180,10 +192,10 @@
     <t xml:space="preserve">descrição do produto</t>
   </si>
   <si>
-    <t>015</t>
-  </si>
-  <si>
-    <t>013-027</t>
+    <t>012</t>
+  </si>
+  <si>
+    <t>013-025</t>
   </si>
   <si>
     <t xml:space="preserve">quantidade de produtos</t>
@@ -192,7 +204,7 @@
     <t>003</t>
   </si>
   <si>
-    <t>027-029</t>
+    <t>026-028</t>
   </si>
   <si>
     <t xml:space="preserve">quantidade de produtos a serem vendidos</t>
@@ -207,7 +219,7 @@
     <t>006</t>
   </si>
   <si>
-    <t>030-035</t>
+    <t>029-34</t>
   </si>
   <si>
     <t>d</t>
@@ -219,7 +231,7 @@
     <t>1</t>
   </si>
   <si>
-    <t xml:space="preserve">registro de dados: "04"</t>
+    <t xml:space="preserve">registro de dados: "01"</t>
   </si>
   <si>
     <t xml:space="preserve">quantidade de registros a inserir</t>
@@ -336,11 +348,13 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="2" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="3" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -351,10 +365,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="4" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf fontId="2" fillId="0" borderId="4" numFmtId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="4" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf fontId="2" fillId="0" borderId="4" numFmtId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf fontId="2" fillId="0" borderId="4" numFmtId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -893,490 +906,515 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
+      <c r="A5" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="D7" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="E7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8" s="8">
+      <c r="A8" s="10">
         <v>1</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="9" t="s">
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="10">
+        <v>1</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="C14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="D14" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="A9" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="10" t="s">
+      <c r="F14" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25">
-      <c r="A10" s="8" t="s">
+      <c r="B15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="10">
+        <v>1</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="A25" s="10">
+        <v>1</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="F26" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25">
-      <c r="A11" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="10" t="s">
+      <c r="B27" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" ht="14.25">
-      <c r="A13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25">
-      <c r="A14" s="8">
-        <v>1</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" ht="14.25">
-      <c r="A15" s="8" t="s">
+      <c r="B28" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25">
-      <c r="A16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25">
-      <c r="A17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25">
-      <c r="A19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" ht="14.25">
-      <c r="A20" s="8">
-        <v>1</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" ht="14.25">
-      <c r="A21" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25">
-      <c r="A22" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" ht="14.25"/>
-    <row r="24" ht="14.25">
-      <c r="A24" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" ht="14.25">
-      <c r="A25" s="8">
-        <v>1</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" ht="14.25">
-      <c r="A26" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" ht="14.25">
-      <c r="A27" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25">
-      <c r="A28" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>60</v>
+      <c r="F28" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E29" s="13" t="s">
+      <c r="A29" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>66</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="30" ht="14.25"/>
     <row r="31" ht="14.25">
-      <c r="A31" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="A31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="B31" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="C31" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="D31" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="14"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
+      <c r="E31" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="15"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="9" t="s">
+      <c r="A32" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="C32" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32" s="14"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
+      <c r="D32" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G32" s="15"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
     </row>
     <row r="33" ht="14.25">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G33" s="14"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
+      <c r="F33" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" s="15"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
     </row>
     <row r="34" ht="14.25"/>
   </sheetData>

</xml_diff>